<commit_message>
example with sum, add a load test with much large number of lines
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="districts" sheetId="1" state="visible" r:id="rId3"/>
@@ -22,7 +22,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
+  <si>
+    <t xml:space="preserve">{{current_row}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{_regions_start_row}}</t>
+  </si>
   <si>
     <t xml:space="preserve">{{name}}</t>
   </si>
@@ -33,6 +39,15 @@
     <t xml:space="preserve">{{_regions_index}}</t>
   </si>
   <si>
+    <t xml:space="preserve">quantity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">settlement</t>
+  </si>
+  <si>
+    <t xml:space="preserve">total fosa</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{range districts}}</t>
   </si>
   <si>
@@ -45,10 +60,19 @@
     <t xml:space="preserve">{{settlement}}</t>
   </si>
   <si>
+    <t xml:space="preserve">{{ fosas | length}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{end}}</t>
   </si>
   <si>
-    <t xml:space="preserve">end group</t>
+    <t xml:space="preserve">{{CONCAT(“=COUNT(E“,_regions_start_row + 1,”:E”, current_row - 1, ”)”)}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{CONCAT(“=SUM(C“,_regions_start_row + 1,”:C”, current_row - 1, ”)”)}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{CONCAT(“=SUM(E“,_regions_start_row + 1,”:E”, current_row - 1, ”)”)}}</t>
   </si>
   <si>
     <t xml:space="preserve">Region</t>
@@ -64,6 +88,9 @@
   </si>
   <si>
     <t xml:space="preserve">Price</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Subsides</t>
   </si>
   <si>
     <t xml:space="preserve">settlement from another sheet</t>
@@ -168,6 +195,9 @@
     <t xml:space="preserve">{{CONCAT(‘=IF(E’, current_row,’="urban", 10, 20)’)}}</t>
   </si>
   <si>
+    <t xml:space="preserve">{{CONCAT(“=E”,current_row,”+F”,current_row)}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">action</t>
   </si>
   <si>
@@ -220,6 +250,12 @@
   </si>
   <si>
     <t xml:space="preserve">ACTIVE_SHEET</t>
+  </si>
+  <si>
+    <t xml:space="preserve">districts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D</t>
   </si>
 </sst>
 </file>
@@ -229,7 +265,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="12">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -250,6 +286,11 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -264,6 +305,11 @@
       <name val="Times New Roman"/>
       <family val="1"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <b val="true"/>
@@ -387,7 +433,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="23">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -396,19 +442,23 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -416,19 +466,47 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="2" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="3" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -436,11 +514,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -520,16 +602,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>5</xdr:col>
-      <xdr:colOff>543960</xdr:colOff>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>658440</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>69840</xdr:rowOff>
+      <xdr:rowOff>51480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>464040</xdr:colOff>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>578520</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>76320</xdr:rowOff>
+      <xdr:rowOff>57600</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -542,8 +624,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4761000" y="69840"/>
-          <a:ext cx="1545840" cy="1469520"/>
+          <a:off x="7315920" y="51480"/>
+          <a:ext cx="1545480" cy="1469160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -569,9 +651,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>739080</xdr:colOff>
+      <xdr:colOff>738720</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1167840</xdr:rowOff>
+      <xdr:rowOff>1167480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -585,7 +667,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12031560" y="23400"/>
-          <a:ext cx="1545840" cy="1469520"/>
+          <a:ext cx="1545480" cy="1469160"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -711,10 +793,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:E10"/>
+  <dimension ref="A1:G10"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -722,66 +804,146 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.45"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.09"/>
   </cols>
   <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F1" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="G2" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F3" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G4" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="3" t="s">
+      <c r="A5" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="C5" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="F5" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
+      <c r="G5" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
+      <c r="A6" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="6"/>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="B7" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="7" t="s">
-        <v>6</v>
+      <c r="G7" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>7</v>
+      <c r="A8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2"/>
-      <c r="E9" s="2" t="s">
-        <v>8</v>
+      <c r="A9" s="3"/>
+      <c r="B9" s="11" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
+      <c r="A10" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -801,10 +963,12 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A2:F12"/>
+  <dimension ref="A2:G12"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C22" activeCellId="0" sqref="C22"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="3" topLeftCell="D4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="bottomLeft" activeCell="D17" activeCellId="0" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -816,99 +980,107 @@
   </cols>
   <sheetData>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="2" t="s">
-        <v>0</v>
+      <c r="A2" s="3" t="s">
+        <v>2</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="93.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="2"/>
+      <c r="A3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="8" t="s">
-        <v>9</v>
-      </c>
-      <c r="B4" s="9" t="s">
+      <c r="A4" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="E4" s="14"/>
+      <c r="F4" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="16" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="F6" s="17"/>
+      <c r="G6" s="18"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="6"/>
+      <c r="D7" s="6"/>
+      <c r="E7" s="6"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="C8" s="3"/>
+      <c r="D8" s="1"/>
+    </row>
+    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D9" s="19" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="D4" s="9" t="s">
-        <v>12</v>
-      </c>
-      <c r="E4" s="9"/>
-      <c r="F4" s="10" t="s">
+      <c r="E9" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" s="10" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="2" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="B9" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D9" s="11" t="s">
-        <v>5</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="2" t="s">
-        <v>7</v>
-      </c>
-    </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="2" t="s">
-        <v>7</v>
+      <c r="A11" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="2" t="s">
-        <v>7</v>
+      <c r="A12" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
@@ -928,10 +1100,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A6" activeCellId="0" sqref="A6"/>
+      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -942,98 +1114,134 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="13" t="s">
-        <v>20</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>22</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>24</v>
+      <c r="A1" s="21" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="21" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="D1" s="21" t="s">
+        <v>33</v>
+      </c>
+      <c r="E1" s="21" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>25</v>
+        <v>35</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>26</v>
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>28</v>
+        <v>38</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="D4" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="D4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>39</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C5" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D5" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="B6" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="C6" s="2" t="s">
-        <v>35</v>
+        <v>44</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>45</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>36</v>
+        <v>46</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="2" t="s">
-        <v>26</v>
+        <v>47</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B9" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C9" s="22" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B10" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C10" s="22" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="B11" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="C11" s="22" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
small integration test, formula transposition
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -21,8 +21,31 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
+  <authors>
+    <author>Unknown Author</author>
+  </authors>
+  <commentList>
+    <comment ref="L7" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <sz val="10"/>
+            <rFont val="Arial"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">equivalent to the formula on the left
+</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
   <si>
     <t xml:space="preserve">{{current_row}}</t>
   </si>
@@ -33,6 +56,12 @@
     <t xml:space="preserve">{{name}}</t>
   </si>
   <si>
+    <t xml:space="preserve">{{sample_url}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{CONCAT(sample_url,”|link name”)}}</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{range regions}}</t>
   </si>
   <si>
@@ -48,6 +77,12 @@
     <t xml:space="preserve">total fosa</t>
   </si>
   <si>
+    <t xml:space="preserve">E + F district</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SUM all district of region</t>
+  </si>
+  <si>
     <t xml:space="preserve">{{range districts}}</t>
   </si>
   <si>
@@ -61,6 +96,9 @@
   </si>
   <si>
     <t xml:space="preserve">{{ fosas | length}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{{CONCAT(“=SUM(E“,current_row,”:F”, current_row, ”)”)}}</t>
   </si>
   <si>
     <t xml:space="preserve">{{end}}</t>
@@ -252,7 +290,13 @@
     <t xml:space="preserve">ACTIVE_SHEET</t>
   </si>
   <si>
+    <t xml:space="preserve">when you edit and save the template the current sheet is the one where you are, this make sure to always have fosas as default active</t>
+  </si>
+  <si>
     <t xml:space="preserve">districts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">fit names for region, district</t>
   </si>
   <si>
     <t xml:space="preserve">D</t>
@@ -262,10 +306,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
-  <fonts count="14">
+  <fonts count="13">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -291,6 +336,13 @@
       <sz val="10"/>
       <name val="Times New Roman"/>
       <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Courier New"/>
+      <family val="3"/>
+      <charset val="1"/>
     </font>
     <font>
       <b val="true"/>
@@ -298,12 +350,6 @@
       <color rgb="FFFAFAFA"/>
       <name val="Arial"/>
       <family val="2"/>
-      <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Times New Roman"/>
-      <family val="1"/>
       <charset val="1"/>
     </font>
     <font>
@@ -345,14 +391,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="10"/>
-      <name val="Courier New"/>
-      <family val="3"/>
-      <charset val="1"/>
-    </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -375,6 +415,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
         <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF43A047"/>
+        <bgColor rgb="FF757575"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFAB91"/>
+        <bgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
@@ -433,7 +485,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="22">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -442,7 +494,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -450,15 +502,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
     <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -470,19 +526,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="6" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -498,15 +550,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -514,15 +562,15 @@
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -574,7 +622,7 @@
       <rgbColor rgb="FFCCFFCC"/>
       <rgbColor rgb="FFFFFF99"/>
       <rgbColor rgb="FF99CCFF"/>
-      <rgbColor rgb="FFFF99CC"/>
+      <rgbColor rgb="FFFFAB91"/>
       <rgbColor rgb="FFCC99FF"/>
       <rgbColor rgb="FFFFCC99"/>
       <rgbColor rgb="FF3366FF"/>
@@ -586,7 +634,7 @@
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
-      <rgbColor rgb="FF339966"/>
+      <rgbColor rgb="FF43A047"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
       <rgbColor rgb="FF993300"/>
@@ -609,9 +657,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>578520</xdr:colOff>
+      <xdr:colOff>577440</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>57600</xdr:rowOff>
+      <xdr:rowOff>56520</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -625,7 +673,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7315920" y="51480"/>
-          <a:ext cx="1545480" cy="1469160"/>
+          <a:ext cx="1544400" cy="1468080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -651,9 +699,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>738720</xdr:colOff>
+      <xdr:colOff>737640</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1167480</xdr:rowOff>
+      <xdr:rowOff>1166400</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -667,7 +715,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12031560" y="23400"/>
-          <a:ext cx="1545480" cy="1469160"/>
+          <a:ext cx="1544400" cy="1468080"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -793,10 +841,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:G10"/>
+  <dimension ref="A1:L10"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B10" activeCellId="0" sqref="B10"/>
+      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -804,7 +852,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="17.17"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="9.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.45"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="23.09"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.09"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -819,6 +867,12 @@
       <c r="B2" s="3" t="s">
         <v>2</v>
       </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
       <c r="F2" s="2" t="s">
         <v>0</v>
       </c>
@@ -827,6 +881,7 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="4"/>
       <c r="F3" s="2" t="s">
         <v>0</v>
       </c>
@@ -836,7 +891,7 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F4" s="2" t="s">
         <v>0</v>
@@ -846,20 +901,20 @@
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="5" t="s">
+      <c r="A5" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="E5" s="5" t="s">
+      <c r="C5" s="6" t="s">
         <v>7</v>
+      </c>
+      <c r="D5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>9</v>
       </c>
       <c r="F5" s="2" t="s">
         <v>0</v>
@@ -867,15 +922,21 @@
       <c r="G5" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="K5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="L5" s="3" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6" s="6"/>
-      <c r="C6" s="6"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="7"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="7"/>
       <c r="F6" s="2" t="s">
         <v>0</v>
       </c>
@@ -885,19 +946,19 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="B7" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="8" t="s">
         <v>2</v>
       </c>
-      <c r="C7" s="8" t="s">
-        <v>10</v>
-      </c>
-      <c r="D7" s="9" t="s">
-        <v>11</v>
-      </c>
-      <c r="E7" s="10" t="s">
-        <v>12</v>
+      <c r="C7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>16</v>
       </c>
       <c r="F7" s="2" t="s">
         <v>0</v>
@@ -905,10 +966,17 @@
       <c r="G7" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="K7" s="11" t="n">
+        <f aca="false">SUM(E7:F7)</f>
+        <v>0</v>
+      </c>
+      <c r="L7" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F8" s="2" t="s">
         <v>0</v>
@@ -919,14 +987,14 @@
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3"/>
-      <c r="B9" s="11" t="s">
-        <v>14</v>
+      <c r="B9" s="3" t="s">
+        <v>19</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>16</v>
+        <v>20</v>
+      </c>
+      <c r="E9" s="3" t="s">
+        <v>21</v>
       </c>
       <c r="F9" s="2" t="s">
         <v>0</v>
@@ -934,10 +1002,14 @@
       <c r="G9" s="2" t="s">
         <v>1</v>
       </c>
+      <c r="L9" s="12" t="n">
+        <f aca="false">SUM(E6:E8)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
       <c r="F10" s="2" t="s">
         <v>0</v>
@@ -954,7 +1026,8 @@
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
-  <drawing r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -989,57 +1062,57 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>20</v>
+        <v>25</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="15" t="s">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="5" t="s">
+      <c r="A6" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B6" s="6" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5" t="s">
-        <v>23</v>
+      <c r="C6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6" t="s">
+        <v>28</v>
       </c>
       <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
+      <c r="G6" s="17"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B7" s="6"/>
-      <c r="C7" s="6"/>
-      <c r="D7" s="6"/>
-      <c r="E7" s="6"/>
+        <v>12</v>
+      </c>
+      <c r="B7" s="7"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="7"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1047,40 +1120,40 @@
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>30</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E9" s="20" t="s">
-        <v>27</v>
-      </c>
-      <c r="F9" s="20" t="s">
-        <v>28</v>
-      </c>
-      <c r="G9" s="10" t="s">
-        <v>29</v>
+      <c r="D9" s="18" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>
@@ -1103,7 +1176,7 @@
   <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B25" activeCellId="0" sqref="B25"/>
+      <selection pane="topLeft" activeCell="E21" activeCellId="0" sqref="E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1114,134 +1187,144 @@
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="21" t="s">
-        <v>30</v>
-      </c>
-      <c r="B1" s="21" t="s">
-        <v>31</v>
-      </c>
-      <c r="C1" s="21" t="s">
-        <v>32</v>
-      </c>
-      <c r="D1" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="E1" s="21" t="s">
-        <v>34</v>
+      <c r="A1" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="B1" s="16" t="s">
+        <v>36</v>
+      </c>
+      <c r="C1" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="E1" s="16" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>37</v>
+        <v>42</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>38</v>
+        <v>43</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>40</v>
+        <v>45</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>39</v>
+        <v>44</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>43</v>
+        <v>48</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>44</v>
+        <v>49</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>45</v>
+        <v>50</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>46</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C9" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B7" s="3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="3"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="22" t="s">
+      <c r="E9" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="C9" s="22" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B10" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C10" s="22" t="s">
-        <v>43</v>
-      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="22" t="s">
-        <v>39</v>
-      </c>
-      <c r="B11" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="C11" s="22" t="s">
-        <v>49</v>
+      <c r="A11" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>56</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add content at the of the xls
</commit_message>
<xml_diff>
--- a/demo.xlsx
+++ b/demo.xlsx
@@ -45,7 +45,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="58">
   <si>
     <t xml:space="preserve">{{current_row}}</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t xml:space="preserve">{{CONCAT(“=SUM(E“,_regions_start_row + 1,”:E”, current_row - 1, ”)”)}}</t>
+  </si>
+  <si>
+    <t xml:space="preserve">This is the end of the listing it’s a work in progress</t>
   </si>
   <si>
     <t xml:space="preserve">Region</t>
@@ -485,7 +488,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -567,10 +570,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -657,9 +656,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>577440</xdr:colOff>
+      <xdr:colOff>577080</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>56520</xdr:rowOff>
+      <xdr:rowOff>56160</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -673,7 +672,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7315920" y="51480"/>
-          <a:ext cx="1544400" cy="1468080"/>
+          <a:ext cx="1544040" cy="1467720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -699,9 +698,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>737640</xdr:colOff>
+      <xdr:colOff>737280</xdr:colOff>
       <xdr:row>2</xdr:row>
-      <xdr:rowOff>1166400</xdr:rowOff>
+      <xdr:rowOff>1166040</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -715,7 +714,7 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="12031560" y="23400"/>
-          <a:ext cx="1544400" cy="1468080"/>
+          <a:ext cx="1544040" cy="1467720"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -841,10 +840,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:L10"/>
+  <dimension ref="A1:L12"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K2" activeCellId="0" sqref="K2"/>
+      <selection pane="topLeft" activeCell="A13" activeCellId="0" sqref="A13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1016,6 +1015,11 @@
       </c>
       <c r="G10" s="2" t="s">
         <v>1</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="1" t="s">
+        <v>22</v>
       </c>
     </row>
   </sheetData>
@@ -1062,23 +1066,23 @@
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="13" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B4" s="14" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="D4" s="14" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E4" s="14"/>
       <c r="F4" s="15" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="G4" s="16" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1096,7 +1100,7 @@
       <c r="C6" s="6"/>
       <c r="D6" s="6"/>
       <c r="E6" s="6" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="F6" s="17"/>
       <c r="G6" s="17"/>
@@ -1112,7 +1116,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="3" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B8" s="3"/>
       <c r="C8" s="3"/>
@@ -1120,10 +1124,10 @@
     </row>
     <row r="9" customFormat="false" ht="15.65" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>2</v>
@@ -1132,13 +1136,13 @@
         <v>14</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -1188,143 +1192,143 @@
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="16" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1" s="16" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="C1" s="16" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D1" s="16" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="E1" s="16" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="D3" s="3"/>
       <c r="E3" s="1" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="D4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="D5" s="3"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="D6" s="1" t="n">
         <v>15</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="19"/>
       <c r="B8" s="20"/>
-      <c r="C8" s="21"/>
+      <c r="C8" s="19"/>
       <c r="D8" s="19"/>
       <c r="E8" s="19"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>

</xml_diff>